<commit_message>
ap promotion product, update database
</commit_message>
<xml_diff>
--- a/DataBeeFit.xlsx
+++ b/DataBeeFit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuphp\OneDrive\Documents\GitHub\BeeFit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D421763-798D-4D4C-8512-FF20D7BDAF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80E3BD8-C11B-44E5-9F6D-6FA21BFA82FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A4" sqref="A4:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,7 +974,7 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{117C104A-D9EB-40EC-8805-E491135436A6}"/>
-    <hyperlink ref="B3:B4" r:id="rId2" display="https://firebasestorage.googleapis.com/v0/b/beefit-e0b4c.appspot.com/o/50bks_3atsb0243_1_a7b95fd2e27f4e178c8d8e82dba217c4_61b7b03e04244f849ba608d7f8d238ef_master.webp?alt=media&amp;token=b7cc80ee-80ee-43c5-bdb5-8dcc7ded72ff" xr:uid="{737D5AE0-8A66-41BA-BECF-07A0367409D3}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{737D5AE0-8A66-41BA-BECF-07A0367409D3}"/>
     <hyperlink ref="B5:B11" r:id="rId3" display="https://firebasestorage.googleapis.com/v0/b/beefit-e0b4c.appspot.com/o/50bks_3atsb0243_1_a7b95fd2e27f4e178c8d8e82dba217c4_61b7b03e04244f849ba608d7f8d238ef_master.webp?alt=media&amp;token=b7cc80ee-80ee-43c5-bdb5-8dcc7ded72ff" xr:uid="{63EA5A4F-1298-435C-AEED-FD568ABEDF6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>